<commit_message>
Made more obvious changes
</commit_message>
<xml_diff>
--- a/144F20/Topic 1/MAT-144 - Working with Formulas and Formatting 20200708.xlsx
+++ b/144F20/Topic 1/MAT-144 - Working with Formulas and Formatting 20200708.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.ketchersid\OneDrive - GCU Employees\Course Materials\git\Teaching\144F20\Topic 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DF38E3-86C3-4AD1-AB8C-C1DD71547BC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:80_{1B225061-A6AF-478E-89D2-89B7DBC9492F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="708" yWindow="444" windowWidth="17436" windowHeight="10824" xr2:uid="{1EF4C19E-4276-4C17-987B-894CE75FA715}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>A(t) = P*(1+r/n)^(n*t)</t>
   </si>
@@ -162,6 +162,37 @@
   </si>
   <si>
     <t>Inflation rate: format as Percentage with 3 decimal places</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Topic 1 DQ 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  For this DQ, you will practice creating Excel formulas from symbolic formulas and formatting cells.  The formulas here are all ones you will be using in this class.
+For each of the symbolic formulas given below in Excel format, you will identify inputs from an example statement and apply the formula in Excel, using appropriate cell references.  Format cells with numeric values as indicated in the "Formatting instructions" sections.
+Pay attention to the legend at the right.  Your entries should be text, numeric, or formulas as indicated by the color-coding in the spreadsheet.</t>
+    </r>
+  </si>
+  <si>
+    <t>Your Name Here</t>
+  </si>
+  <si>
+    <t>Enter Your Name --&gt;</t>
   </si>
 </sst>
 </file>
@@ -172,7 +203,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +222,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -247,7 +286,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -469,11 +508,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -567,6 +643,35 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -594,40 +699,58 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFFFF00"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -645,107 +768,9 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{889DDB35-BACD-4544-95F1-52642DE94671}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="38100" y="63500"/>
-          <a:ext cx="6051550" cy="1739900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
-            <a:t>Topic 1 DQ 1</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>  For this DQ, you will practice creating Excel formulas from symbolic formulas and formatting cells.  The formulas here are all ones you will be using in this class.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>For each of the symbolic formulas given below in Excel format, you will identify inputs from an example statement and apply the formula in Excel, using appropriate cell references.  Format cells with numeric values as indicated in the "Formatting instructions" sections.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>Pay attention to the legend at the right.  Your entries should be text, numeric, or formulas as indicated by the color-coding in the spreadsheet.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{6F856B40-03A3-46C9-B06F-9F93A8571680}">
-  <header guid="{6F856B40-03A3-46C9-B06F-9F93A8571680}" dateTime="2021-01-14T11:15:43" maxSheetId="2" userName="Richard Ketchersid" r:id="rId1">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{13B05A41-09CA-49C0-AA40-A6000A6B45F7}">
+  <header guid="{13B05A41-09CA-49C0-AA40-A6000A6B45F7}" dateTime="2021-02-12T10:45:29" maxSheetId="2" userName="Richard Ketchersid" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -759,7 +784,7 @@
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
-  <userInfo guid="{6F856B40-03A3-46C9-B06F-9F93A8571680}" name="Richard Ketchersid" id="-1739560114" dateTime="2021-01-14T11:15:43"/>
+  <userInfo guid="{13B05A41-09CA-49C0-AA40-A6000A6B45F7}" name="Richard Ketchersid" id="-1739568014" dateTime="2021-02-12T10:45:29"/>
 </users>
 </file>
 
@@ -1060,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E323E0-5480-46DE-B450-C0616525A64F}">
-  <dimension ref="A1:M49"/>
+  <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1078,14 +1103,35 @@
     <col min="9" max="9" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="H2" s="56" t="s">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="H2" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="57"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I2" s="43"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="59"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
       <c r="H3" s="8" t="s">
         <v>17</v>
       </c>
@@ -1093,7 +1139,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="59"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
       <c r="H4" s="10" t="s">
         <v>19</v>
       </c>
@@ -1101,7 +1153,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="59"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
       <c r="H5" s="12" t="s">
         <v>21</v>
       </c>
@@ -1109,7 +1167,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="59"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
       <c r="H6" s="13" t="s">
         <v>23</v>
       </c>
@@ -1117,7 +1181,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="59"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
       <c r="H7" s="14" t="s">
         <v>25</v>
       </c>
@@ -1125,541 +1195,574 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:13" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="51" t="s">
+    <row r="8" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="59"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="59"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+    </row>
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="60"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="61" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="62"/>
+      <c r="C11" s="63" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="64"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="60"/>
+    </row>
+    <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A13" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="53"/>
-    </row>
-    <row r="12" spans="1:13" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="54" t="s">
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="46"/>
+    </row>
+    <row r="14" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="54"/>
-      <c r="C12" s="55" t="s">
+      <c r="B14" s="40"/>
+      <c r="C14" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="55"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="55"/>
-    </row>
-    <row r="13" spans="1:13" ht="44.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="49" t="s">
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+    </row>
+    <row r="15" spans="1:9" ht="44.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="49"/>
-      <c r="C13" s="50" t="s">
+      <c r="B15" s="48"/>
+      <c r="C15" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="50"/>
-      <c r="J13" s="56"/>
-      <c r="K13" s="57"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="43" t="s">
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="6"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="9"/>
-    </row>
-    <row r="15" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="B16" s="53"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="22"/>
+    </row>
+    <row r="17" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="39" t="s">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="G15" s="31"/>
-      <c r="H15" s="32"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="11"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
+      <c r="G17" s="31"/>
+      <c r="H17" s="32"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B18" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C18" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D18" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="33" t="s">
+      <c r="E18" s="1"/>
+      <c r="F18" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="34"/>
-      <c r="H16" s="35"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="11"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="17">
+      <c r="G18" s="34"/>
+      <c r="H18" s="35"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="17">
         <v>4000</v>
       </c>
-      <c r="B17" s="18">
+      <c r="B19" s="18">
         <v>0.123</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C19" s="19">
         <v>4</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D19" s="19">
         <v>5</v>
       </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="33" t="s">
+      <c r="E19" s="1"/>
+      <c r="F19" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="G17" s="34"/>
-      <c r="H17" s="35"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="11"/>
-    </row>
-    <row r="18" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
+      <c r="G19" s="34"/>
+      <c r="H19" s="35"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="16" t="s">
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="25">
-        <f>A17*(1+B17/C17)^(C17*D17)</f>
+      <c r="E20" s="25">
+        <f>A19*(1+B19/C19)^(C19*D19)</f>
         <v>7330.3862815245611</v>
       </c>
-      <c r="F18" s="36" t="s">
+      <c r="F20" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="37"/>
-      <c r="H18" s="38"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="15"/>
-    </row>
-    <row r="19" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="24"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-    </row>
-    <row r="20" spans="1:13" ht="18" x14ac:dyDescent="0.35">
-      <c r="A20" s="51" t="s">
+      <c r="G20" s="37"/>
+      <c r="H20" s="38"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="24"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+    </row>
+    <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="A22" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="52"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="53"/>
-    </row>
-    <row r="21" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="54" t="s">
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="46"/>
+    </row>
+    <row r="23" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="54"/>
-      <c r="C21" s="55" t="s">
+      <c r="B23" s="40"/>
+      <c r="C23" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="55"/>
-    </row>
-    <row r="22" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="49" t="s">
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
+    </row>
+    <row r="24" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="49"/>
-      <c r="C22" s="50" t="s">
+      <c r="B24" s="48"/>
+      <c r="C24" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="50"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="50"/>
-    </row>
-    <row r="23" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="46" t="s">
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
+    </row>
+    <row r="25" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="47"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="6"/>
-    </row>
-    <row r="24" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="B25" s="56"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="6"/>
+    </row>
+    <row r="26" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="39" t="s">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="G24" s="31"/>
-      <c r="H24" s="32"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="16"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="33" t="s">
+      <c r="G26" s="31"/>
+      <c r="H26" s="32"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="G25" s="34"/>
-      <c r="H25" s="35"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="33" t="s">
+      <c r="G27" s="34"/>
+      <c r="H27" s="35"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="26"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="G26" s="34"/>
-      <c r="H26" s="35"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+      <c r="G28" s="34"/>
+      <c r="H28" s="35"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="36" t="s">
+      <c r="B29" s="4"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="G27" s="37"/>
-      <c r="H27" s="38"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="1:13" ht="18" x14ac:dyDescent="0.35">
-      <c r="A29" s="51" t="s">
+      <c r="G29" s="37"/>
+      <c r="H29" s="38"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="A31" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="52"/>
-      <c r="C29" s="52"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="52"/>
-      <c r="H29" s="53"/>
-    </row>
-    <row r="30" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="54" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="54"/>
-      <c r="C30" s="55" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="55"/>
-      <c r="E30" s="55"/>
-      <c r="F30" s="55"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="55"/>
-    </row>
-    <row r="31" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="49" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31" s="49"/>
-      <c r="C31" s="50" t="s">
-        <v>28</v>
-      </c>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="46"/>
     </row>
     <row r="32" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" s="41"/>
-      <c r="C32" s="41"/>
+        <v>5</v>
+      </c>
+      <c r="B32" s="40"/>
+      <c r="C32" s="41" t="s">
+        <v>6</v>
+      </c>
       <c r="D32" s="41"/>
       <c r="E32" s="41"/>
       <c r="F32" s="41"/>
       <c r="G32" s="41"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="6"/>
-    </row>
-    <row r="33" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
+      <c r="H32" s="41"/>
+    </row>
+    <row r="33" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="48"/>
+      <c r="C33" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="47"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="47"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
+    </row>
+    <row r="34" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="50"/>
+      <c r="C34" s="50"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="50"/>
+      <c r="G34" s="50"/>
+      <c r="H34" s="51"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="6"/>
+    </row>
+    <row r="35" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="39" t="s">
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="G33" s="31"/>
-      <c r="H33" s="32"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="16"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="33" t="s">
+      <c r="G35" s="31"/>
+      <c r="H35" s="32"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="16"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="G34" s="34"/>
-      <c r="H34" s="35"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="26"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="33" t="s">
+      <c r="G36" s="34"/>
+      <c r="H36" s="35"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="26"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="G35" s="34"/>
-      <c r="H35" s="35"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+      <c r="G37" s="34"/>
+      <c r="H37" s="35"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="36" t="s">
+      <c r="B38" s="4"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="G36" s="37"/>
-      <c r="H36" s="38"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="6"/>
-    </row>
-    <row r="38" spans="1:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="A38" s="51" t="s">
+      <c r="G38" s="37"/>
+      <c r="H38" s="38"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="A40" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="52"/>
-      <c r="C38" s="52"/>
-      <c r="D38" s="52"/>
-      <c r="E38" s="52"/>
-      <c r="F38" s="52"/>
-      <c r="G38" s="52"/>
-      <c r="H38" s="53"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="21"/>
-    </row>
-    <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="54" t="s">
-        <v>5</v>
-      </c>
-      <c r="B39" s="54"/>
-      <c r="C39" s="55" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="55"/>
-      <c r="E39" s="55"/>
-      <c r="F39" s="55"/>
-      <c r="G39" s="55"/>
-      <c r="H39" s="55"/>
-    </row>
-    <row r="40" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="B40" s="49"/>
-      <c r="C40" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="D40" s="50"/>
-      <c r="E40" s="50"/>
-      <c r="F40" s="50"/>
-      <c r="G40" s="50"/>
-      <c r="H40" s="50"/>
+      <c r="B40" s="45"/>
+      <c r="C40" s="45"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="45"/>
+      <c r="F40" s="45"/>
+      <c r="G40" s="45"/>
+      <c r="H40" s="46"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="21"/>
     </row>
     <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="B41" s="41"/>
-      <c r="C41" s="41"/>
+        <v>5</v>
+      </c>
+      <c r="B41" s="40"/>
+      <c r="C41" s="41" t="s">
+        <v>6</v>
+      </c>
       <c r="D41" s="41"/>
       <c r="E41" s="41"/>
       <c r="F41" s="41"/>
       <c r="G41" s="41"/>
-      <c r="H41" s="42"/>
-      <c r="I41" s="22"/>
-      <c r="J41" s="6"/>
-    </row>
-    <row r="42" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
+      <c r="H41" s="41"/>
+    </row>
+    <row r="42" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42" s="48"/>
+      <c r="C42" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" s="47"/>
+      <c r="E42" s="47"/>
+      <c r="F42" s="47"/>
+      <c r="G42" s="47"/>
+      <c r="H42" s="47"/>
+    </row>
+    <row r="43" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="50"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="50"/>
+      <c r="E43" s="50"/>
+      <c r="F43" s="50"/>
+      <c r="G43" s="50"/>
+      <c r="H43" s="51"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="6"/>
+    </row>
+    <row r="44" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="39" t="s">
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="G42" s="31"/>
-      <c r="H42" s="32"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="16"/>
-      <c r="B43" s="16"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="33" t="s">
+      <c r="G44" s="31"/>
+      <c r="H44" s="32"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="16"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G43" s="34"/>
-      <c r="H43" s="35"/>
-    </row>
-    <row r="44" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="33" t="s">
+      <c r="G45" s="34"/>
+      <c r="H45" s="35"/>
+    </row>
+    <row r="46" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="G44" s="34"/>
-      <c r="H44" s="35"/>
-    </row>
-    <row r="45" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="3" t="s">
+      <c r="G46" s="34"/>
+      <c r="H46" s="35"/>
+    </row>
+    <row r="47" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="4"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="36"/>
-      <c r="G45" s="37"/>
-      <c r="H45" s="38"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="37"/>
+      <c r="H47" s="38"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
     </row>
     <row r="49" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
     </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+    </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C4C65351-310A-417A-BBA6-BF80C4FC9986}">
-      <selection activeCell="G5" sqref="G5"/>
+    <customSheetView guid="{C4C65351-310A-417A-BBA6-BF80C4FC9986}" topLeftCell="A11">
+      <selection activeCell="C11" sqref="C11:E11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
   </customSheetViews>
-  <mergeCells count="26">
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="J13:K13"/>
+  <mergeCells count="28">
+    <mergeCell ref="A43:H43"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:H42"/>
+    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:H32"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:H41"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:H23"/>
     <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A23:H23"/>
-    <mergeCell ref="A32:H32"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="A38:H38"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:H30"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:H39"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="A1:F9"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:E11"/>
   </mergeCells>
+  <conditionalFormatting sqref="A13:H47">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$C$11="Your Name Here"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:E11">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$C$11="Your Name Here"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1673,15 +1776,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010022A2D19B44CEB84096BF732DE0C55A0F" ma:contentTypeVersion="2373" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="893763ede173a64d1d274252a41ae1b2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="b3b59848-949a-4ed4-8036-feb011ce2b52" xmlns:ns3="37d47695-dda2-48a2-87bc-2a1f7ac7fedc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e9673881d9736d6cb1ca37eed258e20f" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1915,6 +2009,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F394CA81-D39C-427F-9EDF-2EA773CCAE31}">
   <ds:schemaRefs>
@@ -1926,14 +2029,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E867C970-83E3-4707-B68A-EABDB3DADE32}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21FFF0FA-A48A-4C31-96BC-D9D70D3D1732}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1951,4 +2046,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E867C970-83E3-4707-B68A-EABDB3DADE32}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added a don't look at Halo preview
</commit_message>
<xml_diff>
--- a/144F20/Topic 1/MAT-144 - Working with Formulas and Formatting 20200708.xlsx
+++ b/144F20/Topic 1/MAT-144 - Working with Formulas and Formatting 20200708.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.ketchersid\OneDrive - GCU Employees\Course Materials\git\Teaching\144F20\Topic 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gcumail-my.sharepoint.com/personal/richard_ketchersid_gcu_edu/Documents/Course Materials/git/Teaching/144F20/Topic 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB6E1A5-FEEE-4982-917F-1B1C2D776D58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:80_{054ACADB-0EE2-410E-A497-58C9C423CB39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11505" xr2:uid="{1EF4C19E-4276-4C17-987B-894CE75FA715}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <customWorkbookViews>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
   <si>
     <t>A(t) = P*(1+r/n)^(n*t)</t>
   </si>
@@ -199,6 +200,9 @@
   </si>
   <si>
     <t>You will see the rest once your name is entered - watch the video!</t>
+  </si>
+  <si>
+    <t>Ignore the Halo preview you must download and open the file in Excel to correctly see the contents.</t>
   </si>
 </sst>
 </file>
@@ -584,7 +588,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -681,6 +685,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -695,21 +741,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -737,32 +768,8 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1131,10 +1138,11 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{58BB145E-3FEF-4F9F-B8AF-2AB3EF951A14}">
-  <header guid="{58BB145E-3FEF-4F9F-B8AF-2AB3EF951A14}" dateTime="2021-04-01T12:23:07" maxSheetId="2" userName="Richard Ketchersid" r:id="rId1">
-    <sheetIdMap count="1">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{8E9BC553-A74A-43E7-9479-964ABCA2D4E3}">
+  <header guid="{8E9BC553-A74A-43E7-9479-964ABCA2D4E3}" dateTime="2022-07-20T13:50:47" maxSheetId="3" userName="Richard Ketchersid" r:id="rId1">
+    <sheetIdMap count="2">
       <sheetId val="1"/>
+      <sheetId val="2"/>
     </sheetIdMap>
   </header>
 </headers>
@@ -1146,7 +1154,7 @@
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
-  <userInfo guid="{58BB145E-3FEF-4F9F-B8AF-2AB3EF951A14}" name="Richard Ketchersid" id="-1739532984" dateTime="2021-04-01T12:23:07"/>
+  <userInfo guid="{8E9BC553-A74A-43E7-9479-964ABCA2D4E3}" name="Richard Ketchersid" id="-1739548868" dateTime="2022-07-20T13:50:47"/>
 </users>
 </file>
 
@@ -1466,34 +1474,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="H2" s="43" t="s">
+      <c r="A2" s="60"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="H2" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="44"/>
+      <c r="I2" s="58"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="51"/>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
+      <c r="A3" s="60"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
       <c r="H3" s="8" t="s">
         <v>17</v>
       </c>
@@ -1502,12 +1510,12 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="51"/>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
+      <c r="A4" s="60"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
       <c r="H4" s="10" t="s">
         <v>19</v>
       </c>
@@ -1516,12 +1524,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="51"/>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
+      <c r="A5" s="60"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
       <c r="H5" s="12" t="s">
         <v>21</v>
       </c>
@@ -1530,12 +1538,12 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="51"/>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
+      <c r="A6" s="60"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
       <c r="H6" s="13" t="s">
         <v>23</v>
       </c>
@@ -1544,12 +1552,12 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="51"/>
-      <c r="B7" s="51"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
+      <c r="A7" s="60"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
       <c r="H7" s="14" t="s">
         <v>25</v>
       </c>
@@ -1558,20 +1566,20 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="51"/>
-      <c r="B8" s="51"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
+      <c r="A8" s="60"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="51"/>
-      <c r="B9" s="51"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
+      <c r="A9" s="60"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="40"/>
@@ -1590,81 +1598,81 @@
       <c r="F11" s="40"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="52" t="s">
+      <c r="A12" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="53"/>
-      <c r="C12" s="54" t="s">
+      <c r="B12" s="62"/>
+      <c r="C12" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="55"/>
-      <c r="E12" s="56"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="65"/>
       <c r="F12" s="40"/>
-      <c r="G12" s="57" t="s">
+      <c r="G12" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="H12" s="57"/>
+      <c r="H12" s="66"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="58" t="s">
+      <c r="A13" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="58"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="58"/>
+      <c r="B13" s="67"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
     </row>
     <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="47"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="54"/>
     </row>
     <row r="15" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="42" t="s">
+      <c r="B15" s="55"/>
+      <c r="C15" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
     </row>
     <row r="16" spans="1:9" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="49"/>
-      <c r="C16" s="48" t="s">
+      <c r="B16" s="50"/>
+      <c r="C16" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="51"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="62" t="s">
+      <c r="A17" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="63"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="64"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="46"/>
       <c r="I17" s="22"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -1749,56 +1757,56 @@
       <c r="M22" s="23"/>
     </row>
     <row r="23" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="46"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="47"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="54"/>
     </row>
     <row r="24" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="41"/>
-      <c r="C24" s="42" t="s">
+      <c r="B24" s="55"/>
+      <c r="C24" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="56"/>
     </row>
     <row r="25" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="49" t="s">
+      <c r="A25" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="49"/>
-      <c r="C25" s="48" t="s">
+      <c r="B25" s="50"/>
+      <c r="C25" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="48"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="51"/>
+      <c r="H25" s="51"/>
     </row>
     <row r="26" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="65" t="s">
+      <c r="A26" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="66"/>
-      <c r="C26" s="66"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="66"/>
-      <c r="F26" s="66"/>
-      <c r="G26" s="66"/>
-      <c r="H26" s="67"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="49"/>
       <c r="I26" s="22"/>
       <c r="J26" s="6"/>
     </row>
@@ -1861,56 +1869,56 @@
       <c r="E31" s="6"/>
     </row>
     <row r="32" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="45" t="s">
+      <c r="A32" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="46"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="46"/>
-      <c r="H32" s="47"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="53"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="54"/>
     </row>
     <row r="33" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="41" t="s">
+      <c r="A33" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="41"/>
-      <c r="C33" s="42" t="s">
+      <c r="B33" s="55"/>
+      <c r="C33" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="42"/>
-      <c r="E33" s="42"/>
-      <c r="F33" s="42"/>
-      <c r="G33" s="42"/>
-      <c r="H33" s="42"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="56"/>
+      <c r="H33" s="56"/>
     </row>
     <row r="34" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="49" t="s">
+      <c r="A34" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="49"/>
-      <c r="C34" s="48" t="s">
+      <c r="B34" s="50"/>
+      <c r="C34" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="D34" s="48"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="48"/>
-      <c r="H34" s="48"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="51"/>
     </row>
     <row r="35" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="59" t="s">
+      <c r="A35" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="60"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="60"/>
-      <c r="F35" s="60"/>
-      <c r="G35" s="60"/>
-      <c r="H35" s="61"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="42"/>
+      <c r="G35" s="42"/>
+      <c r="H35" s="43"/>
       <c r="I35" s="22"/>
       <c r="J35" s="6"/>
     </row>
@@ -1973,58 +1981,58 @@
       <c r="E40" s="6"/>
     </row>
     <row r="41" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="45" t="s">
+      <c r="A41" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="46"/>
-      <c r="C41" s="46"/>
-      <c r="D41" s="46"/>
-      <c r="E41" s="46"/>
-      <c r="F41" s="46"/>
-      <c r="G41" s="46"/>
-      <c r="H41" s="47"/>
+      <c r="B41" s="53"/>
+      <c r="C41" s="53"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="53"/>
+      <c r="F41" s="53"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="54"/>
       <c r="I41" s="20"/>
       <c r="J41" s="21"/>
     </row>
     <row r="42" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="B42" s="41"/>
-      <c r="C42" s="42" t="s">
+      <c r="B42" s="55"/>
+      <c r="C42" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="D42" s="42"/>
-      <c r="E42" s="42"/>
-      <c r="F42" s="42"/>
-      <c r="G42" s="42"/>
-      <c r="H42" s="42"/>
+      <c r="D42" s="56"/>
+      <c r="E42" s="56"/>
+      <c r="F42" s="56"/>
+      <c r="G42" s="56"/>
+      <c r="H42" s="56"/>
     </row>
     <row r="43" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="49" t="s">
+      <c r="A43" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="B43" s="49"/>
-      <c r="C43" s="48" t="s">
+      <c r="B43" s="50"/>
+      <c r="C43" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D43" s="48"/>
-      <c r="E43" s="48"/>
-      <c r="F43" s="48"/>
-      <c r="G43" s="48"/>
-      <c r="H43" s="48"/>
+      <c r="D43" s="51"/>
+      <c r="E43" s="51"/>
+      <c r="F43" s="51"/>
+      <c r="G43" s="51"/>
+      <c r="H43" s="51"/>
     </row>
     <row r="44" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="59" t="s">
+      <c r="A44" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B44" s="60"/>
-      <c r="C44" s="60"/>
-      <c r="D44" s="60"/>
-      <c r="E44" s="60"/>
-      <c r="F44" s="60"/>
-      <c r="G44" s="60"/>
-      <c r="H44" s="61"/>
+      <c r="B44" s="42"/>
+      <c r="C44" s="42"/>
+      <c r="D44" s="42"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="42"/>
+      <c r="G44" s="42"/>
+      <c r="H44" s="43"/>
       <c r="I44" s="22"/>
       <c r="J44" s="6"/>
     </row>
@@ -2105,6 +2113,20 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="A1:F9"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="A13:E13"/>
     <mergeCell ref="A44:H44"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="A26:H26"/>
@@ -2121,20 +2143,6 @@
     <mergeCell ref="C42:H42"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="C25:H25"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:H24"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A23:H23"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="A1:F9"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="A13:E13"/>
   </mergeCells>
   <conditionalFormatting sqref="A14:H48">
     <cfRule type="expression" dxfId="1" priority="2">
@@ -2155,22 +2163,98 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EE4E4FF-485C-4C98-BD2E-90F8BF530D05}">
+  <dimension ref="C5:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="68" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="68"/>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="68"/>
+    </row>
+  </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{C4C65351-310A-417A-BBA6-BF80C4FC9986}" state="hidden">
+      <selection activeCell="C5" sqref="C5:H10"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+  </customSheetViews>
+  <mergeCells count="1">
+    <mergeCell ref="C5:H10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2408,19 +2492,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E867C970-83E3-4707-B68A-EABDB3DADE32}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F394CA81-D39C-427F-9EDF-2EA773CCAE31}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F394CA81-D39C-427F-9EDF-2EA773CCAE31}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E867C970-83E3-4707-B68A-EABDB3DADE32}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>